<commit_message>
Added labels table with explanations for each label.
</commit_message>
<xml_diff>
--- a/Figures/Additional_files/AF2_Labels_North_Sea_review.xlsx
+++ b/Figures/Additional_files/AF2_Labels_North_Sea_review.xlsx
@@ -5,15 +5,22 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrabl/Desktop/NS_review/Paper_publi/Paper_2/Figures/north_sea_review/Figures/Additional_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrabl/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B42C2A3-2BF2-7D45-AD80-79CCDA429B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12808067-CC5E-B24E-BF62-60A71946091A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{FD842753-D541-C546-981C-EB39CC0208C4}"/>
+    <workbookView xWindow="30420" yWindow="2560" windowWidth="35580" windowHeight="21440" xr2:uid="{FD842753-D541-C546-981C-EB39CC0208C4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Labels in SysRev" sheetId="1" r:id="rId1"/>
+    <sheet name="Overview" sheetId="1" r:id="rId1"/>
+    <sheet name="Anthropogenic driver" sheetId="2" r:id="rId2"/>
+    <sheet name="Precision of the driver" sheetId="3" r:id="rId3"/>
+    <sheet name="Analyzed impact" sheetId="4" r:id="rId4"/>
+    <sheet name="Organizational level" sheetId="5" r:id="rId5"/>
+    <sheet name="ICES IV location" sheetId="6" r:id="rId6"/>
+    <sheet name="Spatial dimension" sheetId="7" r:id="rId7"/>
+    <sheet name="Temporal dimension" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="146">
   <si>
     <t>Anthropogenic driver</t>
   </si>
@@ -264,13 +271,223 @@
   </si>
   <si>
     <t>Norwegian coast</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t>Abundance/Density/includes catch volumes as well</t>
+  </si>
+  <si>
+    <t>Age/size/sex ratio etc. size spectrum</t>
+  </si>
+  <si>
+    <t>N of generations, rates of reproduction, mortality/survival/development, age and size at maturity, size at birth, longevity</t>
+  </si>
+  <si>
+    <t>Latitudinal, longitudinal, vertical</t>
+  </si>
+  <si>
+    <t>Degradation/destruction of an habitat</t>
+  </si>
+  <si>
+    <t>Species richness, other biodiversity indicators (e.g., functional diversity)</t>
+  </si>
+  <si>
+    <t>Metabolic processes, energetics, stress, regulation processes, sexual inversion </t>
+  </si>
+  <si>
+    <t>Pollutant concentration in (organs/tissues of) living organisms</t>
+  </si>
+  <si>
+    <t>Timing of seasonal activities (bloom formation, breeding, migration etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes in genes/alleles </t>
+  </si>
+  <si>
+    <t>Gradual accumulation of substances through trophic interactions</t>
+  </si>
+  <si>
+    <t>Bioaccumulation in food web</t>
+  </si>
+  <si>
+    <t>Change in trophic levels, food web structures (e.g. bottom-up/top-down), trophic efficiency, predation/grazing pressures</t>
+  </si>
+  <si>
+    <t>Phosphorus, Carbon, Nitrogen, ratios (e.g. Cd:Ca,Cd:PO4)</t>
+  </si>
+  <si>
+    <t>Increase/decrease of algal blooms</t>
+  </si>
+  <si>
+    <t>Marine heat waves, storm surges, floods, etc.</t>
+  </si>
+  <si>
+    <t>Stratification, currents, warming</t>
+  </si>
+  <si>
+    <t>Grain density, grain size structure, porosity, seafloor structure, geomorphological changes</t>
+  </si>
+  <si>
+    <t>pH, salinity, oxygen concentration, concentration of pollutants</t>
+  </si>
+  <si>
+    <t>pH, salinity, oxygen concentrations, concentration of pollutants; includes particulate organic matter in the water column</t>
+  </si>
+  <si>
+    <t>Geomorphological changes of coastlines</t>
+  </si>
+  <si>
+    <t>Biological toxins (e.g. Paralytic shellfish poisoning)</t>
+  </si>
+  <si>
+    <t>If the driver only was quantified and assessed (e.g. fishing effort, plastic litter)</t>
+  </si>
+  <si>
+    <t>Ingestion of plastic in living organisms</t>
+  </si>
+  <si>
+    <t>If ≧ 3 of the given labels fit</t>
+  </si>
+  <si>
+    <t>If none of the given labels fit</t>
+  </si>
+  <si>
+    <t>Bycatch, beached organisms</t>
+  </si>
+  <si>
+    <t>Non-native species introduction, establishment of populations in an area outside of their natural habitat</t>
+  </si>
+  <si>
+    <t>Changes in climatic conditions (e.g. rising temperatures, sea level rise, extreme weather events)</t>
+  </si>
+  <si>
+    <t>If all five anthropogenic drivers were included in the study</t>
+  </si>
+  <si>
+    <t>Introduction of harmful substances, noise; related to habitat contamination</t>
+  </si>
+  <si>
+    <t>Human activities related to alterations in landscape (e.g. diking, dreding), in energy production (e.g. offshore wind farms, oil and gas extraction)</t>
+  </si>
+  <si>
+    <t>Cultivating, breeding and harvesting aquatic organisms</t>
+  </si>
+  <si>
+    <t>Substances harmful to living organisms and environment</t>
+  </si>
+  <si>
+    <t>Construction and maintenance of civil engineering structures (e.g. offshore windpark, pipelines)</t>
+  </si>
+  <si>
+    <t>Modifications of coastal landscapes (e.g. dikes, dredging)</t>
+  </si>
+  <si>
+    <t>Accidents involving vessels at sea or on waterways</t>
+  </si>
+  <si>
+    <t>Fishing activities (e.g. bottom trawling, blast fishing) causing harm to aquatic habitats, particularly the seafloor, seagrass beds, coral reefs etc.</t>
+  </si>
+  <si>
+    <t>Harvesting of fish and other aquatic organisms for commercial and non-commercial use</t>
+  </si>
+  <si>
+    <t>Unintentional capture of non-target species, e.g. using non-selective fishing gear</t>
+  </si>
+  <si>
+    <t>Illegal, unreported and unregulated fishing</t>
+  </si>
+  <si>
+    <t>Unintentional release of natural gas or other gases from underground storage facilities</t>
+  </si>
+  <si>
+    <t>If human-related impacts are analyzed without mentioning precisely which driver</t>
+  </si>
+  <si>
+    <t>Pharmaceutical drugs or medications</t>
+  </si>
+  <si>
+    <t>Chemical elements with metallic properties</t>
+  </si>
+  <si>
+    <t>Invasive species</t>
+  </si>
+  <si>
+    <t>If no driver was specified</t>
+  </si>
+  <si>
+    <t>Nutrient input into the ecosystem by agriculture, urbanization, industrial purposes</t>
+  </si>
+  <si>
+    <t>If none of the given labels fit (in general)</t>
+  </si>
+  <si>
+    <t>If none of the given labels fit (pollution related)</t>
+  </si>
+  <si>
+    <t>If none of the given labels fit (fishing related)</t>
+  </si>
+  <si>
+    <t>If none of the given labels fit (physical parameters related)</t>
+  </si>
+  <si>
+    <t>Bacteria, viruses, parasites originating from human activities that contaminate aquatic habitats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substances derived from fossil fuels (oil, gas) </t>
+  </si>
+  <si>
+    <t>Extraction of minerals, coal</t>
+  </si>
+  <si>
+    <t>Single individuals are considered (e.g. fish in an experiment (fish tank), dead seabird collected on beaches, contaminated organisms collected individually)</t>
+  </si>
+  <si>
+    <t>Set of individuals of a given species living in an ecosystem</t>
+  </si>
+  <si>
+    <t>Set of populations living in a particular ecosystem and interact with each other; if several species are investigated but individually from each other  = "population" label instead</t>
+  </si>
+  <si>
+    <t>All organisms and the environmental parameters with which they interact (include biotics and abiotics)</t>
+  </si>
+  <si>
+    <t>If not on living organisms</t>
+  </si>
+  <si>
+    <t>Study conducted close to the Norwegian coast and outside the ICES medium areas (1-7)</t>
+  </si>
+  <si>
+    <t>If no area, sampling site was specified</t>
+  </si>
+  <si>
+    <t>If results from 2 or more regions are compared; include only comparisons along the longitudinal/latitudinal gradient; include also studies comparing a North Sea area with an area outside the North Sea</t>
+  </si>
+  <si>
+    <t>If "yes" does not apply</t>
+  </si>
+  <si>
+    <t>If different time periods are compared</t>
+  </si>
+  <si>
+    <t>ICES medium areas (1 to 7, for more details on ICES medium locations see Figure A2.3., ICES (2020) SISP 10 – Manual for the North Sea International Bottom Trawl Surveys. Copenhagen)</t>
+  </si>
+  <si>
+    <t>If all ICES major locations are included (for more details on ICES major areas see Figure A1 (middle), ICES (2024) Definition and rationale for ICES ecoregions. Copenhagen)</t>
+  </si>
+  <si>
+    <t>Utilization of natural resources (e.g. fish, mussels) by humans for commercial, industrial, or subsistence purposes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -284,6 +501,11 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow (Textkörper)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -306,11 +528,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D77F039-644F-634D-98E5-08967144040E}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -992,4 +1216,823 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF04EB40-93B5-5C45-9875-9B0F6CC964BF}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="35.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B17E652-4BB3-E141-AEF2-C2E595566302}">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.1640625" customWidth="1"/>
+    <col min="2" max="2" width="35.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39204839-AB3F-2C4B-AEDA-E1BADFEE50B0}">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.1640625" customWidth="1"/>
+    <col min="2" max="2" width="35.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEEB1446-2093-C749-865E-2D36FDA691B6}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="35.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7E88DD-F53E-DF43-A10A-508F437A2BC2}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="43" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94CBC49C-7CDD-1B48-8ACE-3685AACE6607}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="38.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AABF950-77D8-0244-87D2-A5B19B5046FF}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="35.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>